<commit_message>
Generating test data from Excel File
</commit_message>
<xml_diff>
--- a/MarsQA-1/SpecflowTests/Data/Mars.xlsx
+++ b/MarsQA-1/SpecflowTests/Data/Mars.xlsx
@@ -4,17 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="130" yWindow="550" windowWidth="18880" windowHeight="6740"/>
+    <workbookView xWindow="130" yWindow="550" windowWidth="18880" windowHeight="6740" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
+    <sheet name="Details" sheetId="4" r:id="rId2"/>
+    <sheet name="Language" sheetId="2" r:id="rId3"/>
+    <sheet name="Skills" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>username</t>
   </si>
@@ -26,6 +29,51 @@
   </si>
   <si>
     <t>industryconnect</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Filipino</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>LanguageLevel</t>
+  </si>
+  <si>
+    <t>Fluent</t>
+  </si>
+  <si>
+    <t>Basic</t>
+  </si>
+  <si>
+    <t>Skills</t>
+  </si>
+  <si>
+    <t>C#</t>
+  </si>
+  <si>
+    <t>SkillsLevel</t>
+  </si>
+  <si>
+    <t>Intermediate</t>
+  </si>
+  <si>
+    <t>Java</t>
+  </si>
+  <si>
+    <t>Beginner</t>
+  </si>
+  <si>
+    <t>Availability</t>
+  </si>
+  <si>
+    <t>Hours</t>
+  </si>
+  <si>
+    <t>EarnTarget</t>
   </si>
 </sst>
 </file>
@@ -81,12 +129,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -302,8 +351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1326,4 +1375,125 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="A1:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12.9140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B4" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>